<commit_message>
Small HUD Test Excel Update
</commit_message>
<xml_diff>
--- a/Crawlers/HUD_Crawler_Test_Excel.xlsx
+++ b/Crawlers/HUD_Crawler_Test_Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SectionM8 Business Documents\SectionM8 Fall 2025 Demo\SectionM8-Demo-Fall2025\Crawlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F429BB-84D5-473A-88A8-92BA86BD8DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4BFE33-C6E2-4153-AF9D-259094448AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -715,7 +715,7 @@
   <dimension ref="A1:BH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BB2" sqref="BB2"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,16 +964,16 @@
         <v>75</v>
       </c>
       <c r="U2">
-        <v>1135</v>
+        <v>50</v>
       </c>
       <c r="V2">
-        <v>1033</v>
+        <v>40</v>
       </c>
       <c r="W2" t="s">
         <v>76</v>
       </c>
       <c r="X2">
-        <v>970</v>
+        <v>30</v>
       </c>
       <c r="Y2" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
Small Bug Fix for HUD Crawler
1. AMI $ amount tags in XML test report now populate correctly; same with vacancy rates
</commit_message>
<xml_diff>
--- a/Crawlers/HUD_Crawler_Test_Excel.xlsx
+++ b/Crawlers/HUD_Crawler_Test_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SectionM8 Business Documents\SectionM8 Fall 2025 Demo\SectionM8-Demo-Fall2025\Crawlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4BFE33-C6E2-4153-AF9D-259094448AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBAB35E-2FC6-4544-ACA9-6D1D9BCA2F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
   <si>
     <t>dataset_name</t>
   </si>
@@ -88,9 +88,6 @@
     <t>occupied_units</t>
   </si>
   <si>
-    <t>vacancy_rates</t>
-  </si>
-  <si>
     <t>assisted_units</t>
   </si>
   <si>
@@ -223,18 +220,6 @@
     <t>Region 3</t>
   </si>
   <si>
-    <t>$85,000</t>
-  </si>
-  <si>
-    <t>$24,000</t>
-  </si>
-  <si>
-    <t>$45,000</t>
-  </si>
-  <si>
-    <t>$67,000</t>
-  </si>
-  <si>
     <t>2019-2023</t>
   </si>
   <si>
@@ -250,9 +235,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>6.5%</t>
-  </si>
-  <si>
     <t>HCV</t>
   </si>
   <si>
@@ -332,6 +314,9 @@
   </si>
   <si>
     <t>Run_2025_10_29_001</t>
+  </si>
+  <si>
+    <t>vacancy_rate</t>
   </si>
 </sst>
 </file>
@@ -401,12 +386,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -714,11 +701,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="24" customWidth="1"/>
+    <col min="23" max="23" width="15.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -788,180 +779,180 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>2025</v>
       </c>
       <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>62</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
       </c>
       <c r="F2">
         <v>42091</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H2">
         <v>37980</v>
       </c>
       <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
         <v>65</v>
-      </c>
-      <c r="J2" t="s">
-        <v>66</v>
       </c>
       <c r="K2">
         <v>19406</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="3">
+        <v>85000</v>
+      </c>
+      <c r="M2" s="3">
+        <v>24000</v>
+      </c>
+      <c r="N2">
+        <v>45000</v>
+      </c>
+      <c r="O2">
+        <v>67000</v>
+      </c>
+      <c r="P2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" t="s">
         <v>67</v>
       </c>
-      <c r="M2" t="s">
+      <c r="R2" t="s">
         <v>68</v>
       </c>
-      <c r="N2" t="s">
+      <c r="S2" t="s">
         <v>69</v>
       </c>
-      <c r="O2" t="s">
+      <c r="T2" t="s">
         <v>70</v>
-      </c>
-      <c r="P2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R2" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" t="s">
-        <v>74</v>
-      </c>
-      <c r="T2" t="s">
-        <v>75</v>
       </c>
       <c r="U2">
         <v>50</v>
@@ -969,80 +960,80 @@
       <c r="V2">
         <v>40</v>
       </c>
-      <c r="W2" t="s">
-        <v>76</v>
+      <c r="W2" s="4">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="X2">
         <v>30</v>
       </c>
       <c r="Y2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="Z2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="AA2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AB2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AC2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AD2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AE2">
         <v>921</v>
       </c>
       <c r="AF2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AG2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AH2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="AI2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="AJ2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AK2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="AL2">
         <v>2006</v>
       </c>
       <c r="AM2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AN2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="AO2">
         <v>94</v>
       </c>
       <c r="AP2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="AQ2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="AR2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AS2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AT2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AU2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AV2">
         <v>40.570999999999998</v>
@@ -1057,31 +1048,31 @@
         <v>37964</v>
       </c>
       <c r="AZ2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="BA2" t="b">
         <v>0</v>
       </c>
       <c r="BB2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BH2" t="s">
         <v>97</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>98</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>99</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>101</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>102</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>